<commit_message>
Validation pictures and excel
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/validation/validation results.xlsx
+++ b/Results and scripts_mp/validation/validation results.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="53">
   <si>
     <t>10 sect</t>
   </si>
@@ -70,12 +70,120 @@
   </si>
   <si>
     <t>90 sect</t>
+  </si>
+  <si>
+    <t>elapsed</t>
+  </si>
+  <si>
+    <t>Jakaumakuva</t>
+  </si>
+  <si>
+    <t>Vtot</t>
+  </si>
+  <si>
+    <t>Ntot</t>
+  </si>
+  <si>
+    <t>nukleaatio liian suureen kokoon</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>taustan kasvussa lovia</t>
+  </si>
+  <si>
+    <t>hajoaa (liian pieni Cvap)</t>
+  </si>
+  <si>
+    <t>heittoja nukl ja tausta jakaumassa</t>
+  </si>
+  <si>
+    <t>Yleisesti nukleaatio tapahtuu liian suureen kokoon</t>
+  </si>
+  <si>
+    <t>nukl kasvu portaittain</t>
+  </si>
+  <si>
+    <t>nukl ja tausta kasvu portaittain</t>
+  </si>
+  <si>
+    <t>nukl hyppää taustaan</t>
+  </si>
+  <si>
+    <t>näkyy porras</t>
+  </si>
+  <si>
+    <t>nukl tapahtumassa Ntot laskee</t>
+  </si>
+  <si>
+    <t>Yleisesti näkyy portaittainen kasvu alareunassa</t>
+  </si>
+  <si>
+    <t>porras alas</t>
+  </si>
+  <si>
+    <t>lovi alas</t>
+  </si>
+  <si>
+    <t>todella portaittainen</t>
+  </si>
+  <si>
+    <t>monta lovea nukl tapahtumassa</t>
+  </si>
+  <si>
+    <t>portaittainen nukl</t>
+  </si>
+  <si>
+    <t>portaittainen kasvu</t>
+  </si>
+  <si>
+    <t>monta porrasta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monta lovea </t>
+  </si>
+  <si>
+    <t>sekaista</t>
+  </si>
+  <si>
+    <t>portaat kasvussa</t>
+  </si>
+  <si>
+    <t>isot portaat kasvussa</t>
+  </si>
+  <si>
+    <t>monta lovea</t>
+  </si>
+  <si>
+    <t>nukl katoaa kokonaan kun tapahtuma on ohi</t>
+  </si>
+  <si>
+    <t>Siksakkia</t>
+  </si>
+  <si>
+    <t>portaat</t>
+  </si>
+  <si>
+    <t>Tuntuu hajoavan sitä enmmän mitä enemmän sektioita</t>
+  </si>
+  <si>
+    <t>Lovia ja portaita enemmän</t>
+  </si>
+  <si>
+    <t>Nukl outo viuhkamainen</t>
+  </si>
+  <si>
+    <t>Samankaltaisesti kuin 60 sektiolla ja aiemmilla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,12 +221,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -422,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H66"/>
+  <dimension ref="B2:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,15 +550,32 @@
     <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="23.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="16.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="41.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <v>1</v>
       </c>
@@ -460,8 +591,20 @@
       <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1">
+        <v>1.88697633068916</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C4" s="2">
         <v>2</v>
       </c>
@@ -477,8 +620,20 @@
       <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1">
+        <v>1.28846399315469</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>3</v>
       </c>
@@ -494,8 +649,20 @@
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1">
+        <v>1.4326982347277799</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <v>4</v>
       </c>
@@ -511,8 +678,20 @@
       <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1">
+        <v>1.09901874443161</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <v>5</v>
       </c>
@@ -528,8 +707,20 @@
       <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="1">
+        <v>1.29128948065551</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <v>6</v>
       </c>
@@ -545,8 +736,20 @@
       <c r="G8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1">
+        <v>1.1416364607834499</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <v>7</v>
       </c>
@@ -565,8 +768,20 @@
       <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1">
+        <v>1.76412342858316</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <v>8</v>
       </c>
@@ -585,13 +800,30 @@
       <c r="H10" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <v>1.76288034236827</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <v>1</v>
       </c>
@@ -607,8 +839,20 @@
       <c r="G15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1">
+        <v>6.37268212207261</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <v>2</v>
       </c>
@@ -624,8 +868,20 @@
       <c r="G16" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1">
+        <v>5.5391097501448003</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <v>3</v>
       </c>
@@ -641,8 +897,20 @@
       <c r="G17" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1">
+        <v>5.6405405821466399</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <v>4</v>
       </c>
@@ -658,8 +926,20 @@
       <c r="G18" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1">
+        <v>4.28540983680164</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <v>5</v>
       </c>
@@ -675,8 +955,20 @@
       <c r="G19" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1">
+        <v>6.9607507394053796</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <v>6</v>
       </c>
@@ -692,8 +984,20 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1">
+        <v>6.1191605255342596</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <v>7</v>
       </c>
@@ -712,8 +1016,20 @@
       <c r="H21" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1">
+        <v>7.7416487761886801</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <v>8</v>
       </c>
@@ -732,13 +1048,30 @@
       <c r="H22" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1">
+        <v>7.7070437703613104</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <v>1</v>
       </c>
@@ -754,8 +1087,20 @@
       <c r="G26" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1">
+        <v>18.236905741608702</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <v>2</v>
       </c>
@@ -771,8 +1116,20 @@
       <c r="G27" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1">
+        <v>15.3676587837383</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <v>3</v>
       </c>
@@ -788,8 +1145,20 @@
       <c r="G28" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1">
+        <v>18.622687734562</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <v>4</v>
       </c>
@@ -805,8 +1174,20 @@
       <c r="G29" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1">
+        <v>13.2641667249297</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <v>5</v>
       </c>
@@ -822,8 +1203,20 @@
       <c r="G30" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1">
+        <v>18.063916953117399</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <v>6</v>
       </c>
@@ -839,8 +1232,20 @@
       <c r="G31" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1">
+        <v>17.594250052757399</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <v>7</v>
       </c>
@@ -859,8 +1264,17 @@
       <c r="H32" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1">
+        <v>16.261470485040999</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <v>8</v>
       </c>
@@ -879,13 +1293,22 @@
       <c r="H33" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1">
+        <v>16.228379247772502</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <v>1</v>
       </c>
@@ -901,8 +1324,20 @@
       <c r="G37" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1">
+        <v>31.4236262069257</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <v>2</v>
       </c>
@@ -918,8 +1353,20 @@
       <c r="G38" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1">
+        <v>33.501499657157098</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <v>3</v>
       </c>
@@ -935,8 +1382,20 @@
       <c r="G39" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1">
+        <v>40.685536390418903</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <v>4</v>
       </c>
@@ -952,8 +1411,20 @@
       <c r="G40" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1">
+        <v>23.7989125240615</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <v>5</v>
       </c>
@@ -969,8 +1440,20 @@
       <c r="G41" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1">
+        <v>37.720473014188997</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <v>6</v>
       </c>
@@ -986,8 +1469,20 @@
       <c r="G42" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1">
+        <v>35.400326999665801</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <v>7</v>
       </c>
@@ -1006,8 +1501,20 @@
       <c r="H43" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1">
+        <v>37.425350042943599</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <v>8</v>
       </c>
@@ -1026,13 +1533,25 @@
       <c r="H44" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="1">
+        <v>36.687312182052501</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <v>1</v>
       </c>
@@ -1048,8 +1567,14 @@
       <c r="G48" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="1">
+        <v>151.57512461330001</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <v>2</v>
       </c>
@@ -1065,8 +1590,11 @@
       <c r="G49" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="1">
+        <v>125.739263307854</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <v>3</v>
       </c>
@@ -1082,8 +1610,14 @@
       <c r="G50" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="1">
+        <v>166.17964712515499</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <v>4</v>
       </c>
@@ -1099,8 +1633,11 @@
       <c r="G51" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="1">
+        <v>119.386541763656</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <v>5</v>
       </c>
@@ -1116,8 +1653,11 @@
       <c r="G52" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="1">
+        <v>152.36504625011901</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <v>6</v>
       </c>
@@ -1133,8 +1673,11 @@
       <c r="G53" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="1">
+        <v>152.38883133860099</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <v>7</v>
       </c>
@@ -1153,8 +1696,11 @@
       <c r="H54" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="1">
+        <v>117.415947038626</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C55" s="2">
         <v>8</v>
       </c>
@@ -1173,13 +1719,16 @@
       <c r="H55" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="1">
+        <v>119.93588484583</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C59" s="2">
         <v>1</v>
       </c>
@@ -1195,8 +1744,14 @@
       <c r="G59" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="1">
+        <v>700.36599203475498</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C60" s="2">
         <v>2</v>
       </c>
@@ -1212,8 +1767,11 @@
       <c r="G60" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="1">
+        <v>595.14624992703796</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C61" s="2">
         <v>3</v>
       </c>
@@ -1229,8 +1787,11 @@
       <c r="G61" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="1">
+        <v>802.77881211502302</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C62" s="2">
         <v>4</v>
       </c>
@@ -1246,8 +1807,11 @@
       <c r="G62" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="1">
+        <v>523.49260338044996</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C63" s="2">
         <v>5</v>
       </c>
@@ -1263,8 +1827,11 @@
       <c r="G63" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="1">
+        <v>677.72133445112695</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C64" s="2">
         <v>6</v>
       </c>
@@ -1280,8 +1847,11 @@
       <c r="G64" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="1">
+        <v>677.12246612141098</v>
+      </c>
+    </row>
+    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C65" s="2">
         <v>7</v>
       </c>
@@ -1300,8 +1870,11 @@
       <c r="H65" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="1">
+        <v>582.40919537428294</v>
+      </c>
+    </row>
+    <row r="66" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C66" s="2">
         <v>8</v>
       </c>
@@ -1319,6 +1892,18 @@
       </c>
       <c r="H66" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="I66" s="1">
+        <v>582.36083495881701</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added validation script and results
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/validation/validation results.xlsx
+++ b/Results and scripts_mp/validation/validation results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="56">
   <si>
     <t>10 sect</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>Samankaltaisesti kuin 60 sektiolla ja aiemmilla</t>
+  </si>
+  <si>
+    <t>HUOMIO!!!</t>
+  </si>
+  <si>
+    <t>VIRHEELLISET LAIMENNUKSET!! EIVÄT PIDÄ PAIKKAANSA</t>
+  </si>
+  <si>
+    <t>VAAN OLETUSARVOA ON KÄYTETTY VAHINGOSSA</t>
   </si>
 </sst>
 </file>
@@ -221,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -234,6 +243,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,15 +548,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M66"/>
+  <dimension ref="B1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
@@ -558,6 +571,20 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>

</xml_diff>